<commit_message>
Add Softwares and Cahnge structure
</commit_message>
<xml_diff>
--- a/src/BestPractises-Softwares&Tools.xlsx
+++ b/src/BestPractises-Softwares&Tools.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m-savarian\source\repos\sav68\best-practices-after-new-os\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{958DD733-A74B-48C1-913C-85F356C421A7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EED55DC-BF84-4372-AE77-EBE3ABF9CBCD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{5116FFD8-FF12-4596-A8E8-EA6A71C793EA}"/>
   </bookViews>
@@ -32,10 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="118">
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="112">
   <si>
     <t>Home Users</t>
   </si>
@@ -67,9 +64,6 @@
     <t>Win10</t>
   </si>
   <si>
-    <t>Office Suite</t>
-  </si>
-  <si>
     <t>Microsoft Office Outlook</t>
   </si>
   <si>
@@ -85,45 +79,27 @@
     <t>Microsoft Office Access</t>
   </si>
   <si>
-    <t>Compresor</t>
-  </si>
-  <si>
     <t>WinRar, 7Zip, …</t>
   </si>
   <si>
-    <t>Codec</t>
-  </si>
-  <si>
     <t>K-Lite</t>
   </si>
   <si>
-    <t>CD/DVD Burner</t>
-  </si>
-  <si>
     <t>Power ISO</t>
   </si>
   <si>
-    <t>Download Manager</t>
-  </si>
-  <si>
     <t>IDM</t>
   </si>
   <si>
     <t>uTorrent</t>
   </si>
   <si>
-    <t>Internet Browser</t>
-  </si>
-  <si>
     <t>Chrome</t>
   </si>
   <si>
     <t>FireFox</t>
   </si>
   <si>
-    <t>Messenger</t>
-  </si>
-  <si>
     <t>Telegram</t>
   </si>
   <si>
@@ -133,21 +109,12 @@
     <t>Whatsapp</t>
   </si>
   <si>
-    <t>Fonts</t>
-  </si>
-  <si>
     <t>BFonts</t>
   </si>
   <si>
-    <t>VPN</t>
-  </si>
-  <si>
     <t>CiscoAnyConnect</t>
   </si>
   <si>
-    <t>Remote Tools</t>
-  </si>
-  <si>
     <t>Remote Desktop Manager</t>
   </si>
   <si>
@@ -157,12 +124,6 @@
     <t>UltraViewer</t>
   </si>
   <si>
-    <t>Containers</t>
-  </si>
-  <si>
-    <t>DatabaseTools</t>
-  </si>
-  <si>
     <t>SQL Server</t>
   </si>
   <si>
@@ -187,18 +148,12 @@
     <t>Redis Database Manager</t>
   </si>
   <si>
-    <t>Editor</t>
-  </si>
-  <si>
     <t>VSCode</t>
   </si>
   <si>
     <t>NotePad++</t>
   </si>
   <si>
-    <t>IDE</t>
-  </si>
-  <si>
     <t>Visual Studio</t>
   </si>
   <si>
@@ -211,45 +166,27 @@
     <t>Wireframe Sketcher</t>
   </si>
   <si>
-    <t>MessageBrocker</t>
-  </si>
-  <si>
     <t>RabbitMQ</t>
   </si>
   <si>
     <t>MSMQ</t>
   </si>
   <si>
-    <t>Network Monitor</t>
-  </si>
-  <si>
     <t>Fiddler</t>
   </si>
   <si>
     <t>WireShark</t>
   </si>
   <si>
-    <t>Reporting, BI</t>
-  </si>
-  <si>
     <t>ReportBuilder</t>
   </si>
   <si>
-    <t>Servers Adminsitration</t>
-  </si>
-  <si>
     <t>Windows Admin Center</t>
   </si>
   <si>
-    <t>Source Control</t>
-  </si>
-  <si>
     <t>Git</t>
   </si>
   <si>
-    <t>Virtualization</t>
-  </si>
-  <si>
     <t>Hyper-V</t>
   </si>
   <si>
@@ -262,21 +199,12 @@
     <t>VMWare Vsphere Client</t>
   </si>
   <si>
-    <t>WebAPI Tester</t>
-  </si>
-  <si>
     <t>PostMan</t>
   </si>
   <si>
-    <t>WebServer</t>
-  </si>
-  <si>
     <t>Nginx</t>
   </si>
   <si>
-    <t>Graphic</t>
-  </si>
-  <si>
     <t>Adobe PhotoShop</t>
   </si>
   <si>
@@ -373,9 +301,6 @@
     <t>StimuleSoft Designer</t>
   </si>
   <si>
-    <t>Mobile Tools</t>
-  </si>
-  <si>
     <t>Framework Name</t>
   </si>
   <si>
@@ -385,7 +310,64 @@
     <t>BI Developer</t>
   </si>
   <si>
-    <t>Graph</t>
+    <t>GitHub Desktop</t>
+  </si>
+  <si>
+    <t>Adobe XE</t>
+  </si>
+  <si>
+    <t>Xampp</t>
+  </si>
+  <si>
+    <t>Wamp</t>
+  </si>
+  <si>
+    <t>Lampp</t>
+  </si>
+  <si>
+    <t>Visio</t>
+  </si>
+  <si>
+    <t>OneNote</t>
+  </si>
+  <si>
+    <t>Project Management</t>
+  </si>
+  <si>
+    <t>Microsoft Project</t>
+  </si>
+  <si>
+    <t>Oracle Primavera (P6)</t>
+  </si>
+  <si>
+    <t>NuGet Package Explorer</t>
+  </si>
+  <si>
+    <t>PuTTy</t>
+  </si>
+  <si>
+    <t>Basic Tools</t>
+  </si>
+  <si>
+    <t>Network Tools</t>
+  </si>
+  <si>
+    <t>Virtualization Tools</t>
+  </si>
+  <si>
+    <t>Developer Tools</t>
+  </si>
+  <si>
+    <t>Data Tools</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> GId</t>
+  </si>
+  <si>
+    <t>Design Tools</t>
+  </si>
+  <si>
+    <t>Designer</t>
   </si>
 </sst>
 </file>
@@ -460,80 +442,23 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="15">
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <b/>
@@ -577,6 +502,63 @@
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -591,27 +573,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7344C024-51DA-40F2-8937-22646FE5926D}" name="Table1" displayName="Table1" ref="A2:O69" totalsRowShown="0">
-  <autoFilter ref="A2:O69" xr:uid="{273241F8-2B03-4975-8B03-92D3E2424227}"/>
-  <sortState ref="A3:O69">
-    <sortCondition ref="A2:A69"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7344C024-51DA-40F2-8937-22646FE5926D}" name="Table1" displayName="Table1" ref="A2:O76" totalsRowShown="0">
+  <autoFilter ref="A2:O76" xr:uid="{273241F8-2B03-4975-8B03-92D3E2424227}"/>
+  <sortState ref="A3:O76">
+    <sortCondition ref="A2:A76"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="11" xr3:uid="{73182DE8-4519-4C98-81DD-7CB53560BD58}" name=" " dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{B2F26F45-D017-4AEE-9258-B2E0FED3475F}" name="  Category" dataDxfId="3"/>
-    <tableColumn id="14" xr3:uid="{475D00EE-DBF3-4509-B199-766ACE012349}" name="Platform" dataDxfId="1"/>
-    <tableColumn id="12" xr3:uid="{FECD2DAB-AE55-4A73-9EA3-393E66C65DED}" name="Cost" dataDxfId="2"/>
-    <tableColumn id="1" xr3:uid="{DBCCBA0F-2CC0-41FC-B36B-D32C783A1346}" name="Softwares" dataDxfId="5"/>
-    <tableColumn id="13" xr3:uid="{55A75063-0F04-4048-A7BC-5431239C2401}" name="Home Users" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{CB83FC61-5871-4519-895B-0CED840B1379}" name="Office Users" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{FF70DF90-2E81-4F95-9AB3-2724E7509C70}" name="Accountant Users" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{74804E52-9F80-46CE-A575-5114D5B9F303}" name=".Net Developers" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{CF1DB752-52A5-4699-9735-CDBCC0C5F30B}" name="Java Developers" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{C1CEC3D5-8BF0-40AB-9FB9-8FB6429B4D41}" name="Web Develoeprs" dataDxfId="10"/>
-    <tableColumn id="15" xr3:uid="{15D396CA-877E-4B01-85C0-C69A4CF9ECF6}" name="BI Developer" dataDxfId="0"/>
-    <tableColumn id="7" xr3:uid="{E487DF67-D708-4530-8F4D-881AEFA4F1F2}" name="Graph" dataDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{1AA01AC2-D46F-49D6-BDE3-8A1D305E0461}" name="Network Admin" dataDxfId="8"/>
-    <tableColumn id="9" xr3:uid="{7CA4C263-95CB-4552-8825-A73CBBFC7E2D}" name="SysAdmin" dataDxfId="7"/>
+    <tableColumn id="11" xr3:uid="{73182DE8-4519-4C98-81DD-7CB53560BD58}" name=" GId" dataDxfId="14"/>
+    <tableColumn id="10" xr3:uid="{B2F26F45-D017-4AEE-9258-B2E0FED3475F}" name="  Category" dataDxfId="13"/>
+    <tableColumn id="14" xr3:uid="{475D00EE-DBF3-4509-B199-766ACE012349}" name="Platform" dataDxfId="12"/>
+    <tableColumn id="12" xr3:uid="{FECD2DAB-AE55-4A73-9EA3-393E66C65DED}" name="Cost" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{DBCCBA0F-2CC0-41FC-B36B-D32C783A1346}" name="Softwares" dataDxfId="10"/>
+    <tableColumn id="13" xr3:uid="{55A75063-0F04-4048-A7BC-5431239C2401}" name="Home Users" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{CB83FC61-5871-4519-895B-0CED840B1379}" name="Office Users" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{FF70DF90-2E81-4F95-9AB3-2724E7509C70}" name="Accountant Users" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{74804E52-9F80-46CE-A575-5114D5B9F303}" name=".Net Developers" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{CF1DB752-52A5-4699-9735-CDBCC0C5F30B}" name="Java Developers" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{C1CEC3D5-8BF0-40AB-9FB9-8FB6429B4D41}" name="Web Develoeprs" dataDxfId="5"/>
+    <tableColumn id="15" xr3:uid="{15D396CA-877E-4B01-85C0-C69A4CF9ECF6}" name="BI Developer" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{E487DF67-D708-4530-8F4D-881AEFA4F1F2}" name="Designer" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{1AA01AC2-D46F-49D6-BDE3-8A1D305E0461}" name="Network Admin" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{7CA4C263-95CB-4552-8825-A73CBBFC7E2D}" name="SysAdmin" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -936,16 +918,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E39B217-E170-403E-8CBC-8ED6F3D0F392}">
-  <dimension ref="A1:O69"/>
+  <dimension ref="A1:O76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" topLeftCell="K1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <pane xSplit="5" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10" style="1" customWidth="1"/>
     <col min="2" max="2" width="22.28515625" customWidth="1"/>
     <col min="3" max="3" width="15.140625" customWidth="1"/>
     <col min="4" max="4" width="10.28515625" customWidth="1"/>
@@ -955,193 +937,237 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
+      <c r="A1" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
       <c r="L1" s="7"/>
-      <c r="M1" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
+      <c r="M1" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
     </row>
     <row r="2" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="L2" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="N2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="N2" s="4" t="s">
+      <c r="O2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="O2" s="4" t="s">
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
+      <c r="C3" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="O3" s="6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
-        <v>1</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="10">
-        <v>1</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="10">
-        <v>2</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="5"/>
+      <c r="F6" s="6"/>
       <c r="G6" s="6" t="s">
-        <v>95</v>
+        <v>71</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -1153,24 +1179,24 @@
       <c r="O6" s="6"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="10">
+      <c r="A7" s="8">
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="5"/>
+      <c r="F7" s="6"/>
       <c r="G7" s="6" t="s">
-        <v>95</v>
+        <v>71</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -1182,24 +1208,24 @@
       <c r="O7" s="6"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="10">
+      <c r="A8" s="8">
         <v>2</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="11" t="s">
         <v>104</v>
       </c>
+      <c r="C8" s="9" t="s">
+        <v>80</v>
+      </c>
       <c r="D8" s="5" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="5"/>
+        <v>12</v>
+      </c>
+      <c r="F8" s="6"/>
       <c r="G8" s="6" t="s">
-        <v>95</v>
+        <v>71</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -1211,22 +1237,22 @@
       <c r="O8" s="6"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="10">
+      <c r="A9" s="8">
         <v>2</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="11" t="s">
         <v>104</v>
       </c>
+      <c r="C9" s="9" t="s">
+        <v>80</v>
+      </c>
       <c r="D9" s="5" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="F9" s="6"/>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -1238,22 +1264,22 @@
       <c r="O9" s="6"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="10">
+      <c r="A10" s="8">
         <v>2</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="11" t="s">
         <v>104</v>
       </c>
+      <c r="C10" s="9" t="s">
+        <v>80</v>
+      </c>
       <c r="D10" s="5" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="5"/>
+        <v>14</v>
+      </c>
+      <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -1265,24 +1291,24 @@
       <c r="O10" s="6"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="10">
-        <v>3</v>
+      <c r="A11" s="8">
+        <v>2</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="11" t="s">
         <v>104</v>
       </c>
+      <c r="C11" s="9" t="s">
+        <v>80</v>
+      </c>
       <c r="D11" s="5" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="5"/>
+        <v>15</v>
+      </c>
+      <c r="F11" s="6"/>
       <c r="G11" s="6" t="s">
-        <v>95</v>
+        <v>71</v>
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -1294,22 +1320,22 @@
       <c r="O11" s="6"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="10">
-        <v>4</v>
+      <c r="A12" s="8">
+        <v>2</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="11" t="s">
         <v>104</v>
       </c>
+      <c r="C12" s="9" t="s">
+        <v>80</v>
+      </c>
       <c r="D12" s="5" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" s="5"/>
+        <v>16</v>
+      </c>
+      <c r="F12" s="6"/>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
@@ -1321,22 +1347,22 @@
       <c r="O12" s="6"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="10">
-        <v>5</v>
+      <c r="A13" s="8">
+        <v>2</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="11" t="s">
         <v>104</v>
       </c>
+      <c r="C13" s="9" t="s">
+        <v>80</v>
+      </c>
       <c r="D13" s="5" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
@@ -1348,22 +1374,22 @@
       <c r="O13" s="6"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="10">
-        <v>6</v>
+      <c r="A14" s="8">
+        <v>2</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="11" t="s">
         <v>104</v>
       </c>
+      <c r="C14" s="9" t="s">
+        <v>80</v>
+      </c>
       <c r="D14" s="5" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F14" s="5"/>
+        <v>18</v>
+      </c>
+      <c r="F14" s="6"/>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
@@ -1375,22 +1401,22 @@
       <c r="O14" s="6"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="10">
-        <v>6</v>
+      <c r="A15" s="8">
+        <v>2</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="11" t="s">
         <v>104</v>
       </c>
+      <c r="C15" s="9" t="s">
+        <v>80</v>
+      </c>
       <c r="D15" s="5" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F15" s="5"/>
+        <v>19</v>
+      </c>
+      <c r="F15" s="6"/>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
@@ -1402,24 +1428,24 @@
       <c r="O15" s="6"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="10">
-        <v>7</v>
+      <c r="A16" s="8">
+        <v>2</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" s="11" t="s">
         <v>104</v>
       </c>
+      <c r="C16" s="9" t="s">
+        <v>80</v>
+      </c>
       <c r="D16" s="5" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F16" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="F16" s="6"/>
       <c r="G16" s="6" t="s">
-        <v>95</v>
+        <v>71</v>
       </c>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
@@ -1431,24 +1457,24 @@
       <c r="O16" s="6"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="10">
-        <v>7</v>
+      <c r="A17" s="8">
+        <v>2</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="11" t="s">
         <v>104</v>
       </c>
+      <c r="C17" s="9" t="s">
+        <v>80</v>
+      </c>
       <c r="D17" s="5" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F17" s="5"/>
+        <v>21</v>
+      </c>
+      <c r="F17" s="6"/>
       <c r="G17" s="6" t="s">
-        <v>95</v>
+        <v>71</v>
       </c>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
@@ -1460,22 +1486,22 @@
       <c r="O17" s="6"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="10">
-        <v>8</v>
+      <c r="A18" s="8">
+        <v>2</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="11" t="s">
         <v>104</v>
       </c>
+      <c r="C18" s="9" t="s">
+        <v>80</v>
+      </c>
       <c r="D18" s="5" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F18" s="5"/>
+        <v>22</v>
+      </c>
+      <c r="F18" s="6"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
@@ -1487,22 +1513,22 @@
       <c r="O18" s="6"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="10">
-        <v>8</v>
+      <c r="A19" s="8">
+        <v>2</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" s="11" t="s">
         <v>104</v>
       </c>
+      <c r="C19" s="9" t="s">
+        <v>80</v>
+      </c>
       <c r="D19" s="5" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F19" s="5"/>
+        <v>23</v>
+      </c>
+      <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
@@ -1514,22 +1540,22 @@
       <c r="O19" s="6"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="10">
-        <v>8</v>
+      <c r="A20" s="8">
+        <v>2</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" s="11" t="s">
         <v>104</v>
       </c>
+      <c r="C20" s="9" t="s">
+        <v>80</v>
+      </c>
       <c r="D20" s="5" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F20" s="5"/>
+        <v>24</v>
+      </c>
+      <c r="F20" s="6"/>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
@@ -1541,24 +1567,24 @@
       <c r="O20" s="6"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="10">
-        <v>9</v>
+      <c r="A21" s="8">
+        <v>2</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" s="11" t="s">
         <v>104</v>
       </c>
+      <c r="C21" s="9" t="s">
+        <v>80</v>
+      </c>
       <c r="D21" s="5" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F21" s="5"/>
+        <v>25</v>
+      </c>
+      <c r="F21" s="6"/>
       <c r="G21" s="6" t="s">
-        <v>95</v>
+        <v>71</v>
       </c>
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
@@ -1570,22 +1596,22 @@
       <c r="O21" s="6"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="10">
-        <v>10</v>
+      <c r="A22" s="8">
+        <v>2</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C22" s="11" t="s">
         <v>104</v>
       </c>
+      <c r="C22" s="9" t="s">
+        <v>80</v>
+      </c>
       <c r="D22" s="5" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F22" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="F22" s="6"/>
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
@@ -1597,22 +1623,22 @@
       <c r="O22" s="6"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="10">
-        <v>11</v>
+      <c r="A23" s="8">
+        <v>2</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23" s="11" t="s">
         <v>104</v>
       </c>
+      <c r="C23" s="9" t="s">
+        <v>80</v>
+      </c>
       <c r="D23" s="5" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F23" s="5"/>
+        <v>59</v>
+      </c>
+      <c r="F23" s="6"/>
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
@@ -1624,22 +1650,22 @@
       <c r="O23" s="6"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="10">
-        <v>11</v>
+      <c r="A24" s="8">
+        <v>2</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C24" s="11" t="s">
         <v>104</v>
       </c>
+      <c r="C24" s="9" t="s">
+        <v>80</v>
+      </c>
       <c r="D24" s="5" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F24" s="5"/>
+        <v>98</v>
+      </c>
+      <c r="F24" s="6"/>
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
@@ -1651,22 +1677,22 @@
       <c r="O24" s="6"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="10">
-        <v>11</v>
+      <c r="A25" s="8">
+        <v>10</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>104</v>
+        <v>99</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F25" s="5"/>
+        <v>100</v>
+      </c>
+      <c r="F25" s="6"/>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
@@ -1678,20 +1704,22 @@
       <c r="O25" s="6"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="10"/>
+      <c r="A26" s="8">
+        <v>10</v>
+      </c>
       <c r="B26" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>104</v>
+        <v>99</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="F26" s="5"/>
+        <v>101</v>
+      </c>
+      <c r="F26" s="6"/>
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
       <c r="I26" s="6"/>
@@ -1703,20 +1731,22 @@
       <c r="O26" s="6"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="10"/>
+      <c r="A27" s="8">
+        <v>11</v>
+      </c>
       <c r="B27" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>104</v>
+        <v>105</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F27" s="5"/>
+        <v>27</v>
+      </c>
+      <c r="F27" s="6"/>
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
       <c r="I27" s="6"/>
@@ -1728,20 +1758,22 @@
       <c r="O27" s="6"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="10"/>
+      <c r="A28" s="8">
+        <v>11</v>
+      </c>
       <c r="B28" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>104</v>
+        <v>105</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F28" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="F28" s="6"/>
       <c r="G28" s="6"/>
       <c r="H28" s="6"/>
       <c r="I28" s="6"/>
@@ -1753,20 +1785,22 @@
       <c r="O28" s="6"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="10"/>
+      <c r="A29" s="8">
+        <v>11</v>
+      </c>
       <c r="B29" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>104</v>
+        <v>105</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F29" s="5"/>
+        <v>29</v>
+      </c>
+      <c r="F29" s="6"/>
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
       <c r="I29" s="6"/>
@@ -1778,18 +1812,22 @@
       <c r="O29" s="6"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="10"/>
+      <c r="A30" s="8">
+        <v>11</v>
+      </c>
       <c r="B30" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>104</v>
+        <v>105</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="E30" s="3"/>
-      <c r="F30" s="5"/>
+        <v>67</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F30" s="6"/>
       <c r="G30" s="6"/>
       <c r="H30" s="6"/>
       <c r="I30" s="6"/>
@@ -1801,20 +1839,20 @@
       <c r="O30" s="6"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="10"/>
+      <c r="A31" s="8">
+        <v>11</v>
+      </c>
       <c r="B31" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>104</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="C31" s="9"/>
       <c r="D31" s="5" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F31" s="5"/>
+        <v>103</v>
+      </c>
+      <c r="F31" s="6"/>
       <c r="G31" s="6"/>
       <c r="H31" s="6"/>
       <c r="I31" s="6"/>
@@ -1826,20 +1864,22 @@
       <c r="O31" s="6"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="10"/>
+      <c r="A32" s="8">
+        <v>11</v>
+      </c>
       <c r="B32" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>104</v>
+        <v>105</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>81</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F32" s="5"/>
+        <v>49</v>
+      </c>
+      <c r="F32" s="6"/>
       <c r="G32" s="6"/>
       <c r="H32" s="6"/>
       <c r="I32" s="6"/>
@@ -1851,20 +1891,22 @@
       <c r="O32" s="6"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A33" s="10"/>
+      <c r="A33" s="8">
+        <v>12</v>
+      </c>
       <c r="B33" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>104</v>
+        <v>106</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F33" s="5"/>
+        <v>68</v>
+      </c>
+      <c r="F33" s="6"/>
       <c r="G33" s="6"/>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
@@ -1876,20 +1918,22 @@
       <c r="O33" s="6"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A34" s="10"/>
+      <c r="A34" s="8">
+        <v>12</v>
+      </c>
       <c r="B34" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>104</v>
+        <v>106</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>81</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F34" s="5"/>
+        <v>51</v>
+      </c>
+      <c r="F34" s="6"/>
       <c r="G34" s="6"/>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
@@ -1901,20 +1945,22 @@
       <c r="O34" s="6"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A35" s="10"/>
+      <c r="A35" s="8">
+        <v>12</v>
+      </c>
       <c r="B35" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C35" s="11" t="s">
-        <v>104</v>
+        <v>106</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F35" s="5"/>
+        <v>52</v>
+      </c>
+      <c r="F35" s="6"/>
       <c r="G35" s="6"/>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
@@ -1926,20 +1972,22 @@
       <c r="O35" s="6"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A36" s="10"/>
+      <c r="A36" s="8">
+        <v>12</v>
+      </c>
       <c r="B36" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>104</v>
+        <v>106</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F36" s="5"/>
+        <v>53</v>
+      </c>
+      <c r="F36" s="6"/>
       <c r="G36" s="6"/>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
@@ -1951,20 +1999,22 @@
       <c r="O36" s="6"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A37" s="10"/>
+      <c r="A37" s="8">
+        <v>12</v>
+      </c>
       <c r="B37" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C37" s="11" t="s">
-        <v>104</v>
+        <v>106</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F37" s="5"/>
+        <v>54</v>
+      </c>
+      <c r="F37" s="6"/>
       <c r="G37" s="6"/>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
@@ -1976,20 +2026,22 @@
       <c r="O37" s="6"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A38" s="10"/>
+      <c r="A38" s="8">
+        <v>13</v>
+      </c>
       <c r="B38" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C38" s="11" t="s">
-        <v>104</v>
+        <v>107</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F38" s="5"/>
+        <v>50</v>
+      </c>
+      <c r="F38" s="6"/>
       <c r="G38" s="6"/>
       <c r="H38" s="6"/>
       <c r="I38" s="6"/>
@@ -2001,20 +2053,22 @@
       <c r="O38" s="6"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A39" s="10"/>
+      <c r="A39" s="8">
+        <v>13</v>
+      </c>
       <c r="B39" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C39" s="11" t="s">
-        <v>104</v>
+        <v>107</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F39" s="5"/>
+        <v>92</v>
+      </c>
+      <c r="F39" s="6"/>
       <c r="G39" s="6"/>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
@@ -2026,20 +2080,22 @@
       <c r="O39" s="6"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A40" s="10"/>
+      <c r="A40" s="8">
+        <v>13</v>
+      </c>
       <c r="B40" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C40" s="11" t="s">
-        <v>104</v>
+        <v>107</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F40" s="5"/>
+        <v>40</v>
+      </c>
+      <c r="F40" s="6"/>
       <c r="G40" s="6"/>
       <c r="H40" s="6"/>
       <c r="I40" s="6"/>
@@ -2051,20 +2107,22 @@
       <c r="O40" s="6"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A41" s="10"/>
+      <c r="A41" s="8">
+        <v>13</v>
+      </c>
       <c r="B41" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C41" s="11" t="s">
-        <v>104</v>
+        <v>107</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F41" s="5"/>
+        <v>41</v>
+      </c>
+      <c r="F41" s="6"/>
       <c r="G41" s="6"/>
       <c r="H41" s="6"/>
       <c r="I41" s="6"/>
@@ -2076,20 +2134,22 @@
       <c r="O41" s="6"/>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A42" s="10"/>
+      <c r="A42" s="8">
+        <v>13</v>
+      </c>
       <c r="B42" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C42" s="11" t="s">
-        <v>104</v>
+        <v>107</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F42" s="5"/>
+        <v>42</v>
+      </c>
+      <c r="F42" s="6"/>
       <c r="G42" s="6"/>
       <c r="H42" s="6"/>
       <c r="I42" s="6"/>
@@ -2101,20 +2161,22 @@
       <c r="O42" s="6"/>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A43" s="10"/>
+      <c r="A43" s="8">
+        <v>13</v>
+      </c>
       <c r="B43" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C43" s="11" t="s">
-        <v>105</v>
+        <v>107</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F43" s="5"/>
+        <v>38</v>
+      </c>
+      <c r="F43" s="6"/>
       <c r="G43" s="6"/>
       <c r="H43" s="6"/>
       <c r="I43" s="6"/>
@@ -2126,20 +2188,22 @@
       <c r="O43" s="6"/>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A44" s="10"/>
+      <c r="A44" s="8">
+        <v>13</v>
+      </c>
       <c r="B44" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C44" s="11" t="s">
-        <v>104</v>
+        <v>107</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="F44" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F44" s="6"/>
       <c r="G44" s="6"/>
       <c r="H44" s="6"/>
       <c r="I44" s="6"/>
@@ -2151,20 +2215,22 @@
       <c r="O44" s="6"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A45" s="10"/>
+      <c r="A45" s="8">
+        <v>13</v>
+      </c>
       <c r="B45" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C45" s="11" t="s">
-        <v>104</v>
+        <v>107</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F45" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F45" s="6"/>
       <c r="G45" s="6"/>
       <c r="H45" s="6"/>
       <c r="I45" s="6"/>
@@ -2176,20 +2242,22 @@
       <c r="O45" s="6"/>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A46" s="10"/>
+      <c r="A46" s="8">
+        <v>13</v>
+      </c>
       <c r="B46" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C46" s="11" t="s">
-        <v>105</v>
+        <v>107</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>81</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="F46" s="5"/>
+        <v>45</v>
+      </c>
+      <c r="F46" s="6"/>
       <c r="G46" s="6"/>
       <c r="H46" s="6"/>
       <c r="I46" s="6"/>
@@ -2201,20 +2269,22 @@
       <c r="O46" s="6"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A47" s="10"/>
+      <c r="A47" s="8">
+        <v>13</v>
+      </c>
       <c r="B47" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C47" s="11" t="s">
-        <v>104</v>
+        <v>107</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="F47" s="5"/>
+        <v>55</v>
+      </c>
+      <c r="F47" s="6"/>
       <c r="G47" s="6"/>
       <c r="H47" s="6"/>
       <c r="I47" s="6"/>
@@ -2226,20 +2296,22 @@
       <c r="O47" s="6"/>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A48" s="10"/>
+      <c r="A48" s="8">
+        <v>13</v>
+      </c>
       <c r="B48" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C48" s="11" t="s">
-        <v>104</v>
+        <v>107</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="F48" s="5"/>
+        <v>56</v>
+      </c>
+      <c r="F48" s="6"/>
       <c r="G48" s="6"/>
       <c r="H48" s="6"/>
       <c r="I48" s="6"/>
@@ -2251,20 +2323,22 @@
       <c r="O48" s="6"/>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A49" s="10"/>
+      <c r="A49" s="8">
+        <v>13</v>
+      </c>
       <c r="B49" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C49" s="11" t="s">
-        <v>105</v>
+        <v>107</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="F49" s="5"/>
+        <v>94</v>
+      </c>
+      <c r="F49" s="6"/>
       <c r="G49" s="6"/>
       <c r="H49" s="6"/>
       <c r="I49" s="6"/>
@@ -2276,20 +2350,22 @@
       <c r="O49" s="6"/>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A50" s="10"/>
+      <c r="A50" s="8">
+        <v>13</v>
+      </c>
       <c r="B50" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C50" s="11" t="s">
-        <v>105</v>
+        <v>107</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="F50" s="5"/>
+        <v>95</v>
+      </c>
+      <c r="F50" s="6"/>
       <c r="G50" s="6"/>
       <c r="H50" s="6"/>
       <c r="I50" s="6"/>
@@ -2301,20 +2377,22 @@
       <c r="O50" s="6"/>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A51" s="10"/>
+      <c r="A51" s="8">
+        <v>13</v>
+      </c>
       <c r="B51" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C51" s="11" t="s">
-        <v>104</v>
+        <v>107</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F51" s="5"/>
+        <v>96</v>
+      </c>
+      <c r="F51" s="6"/>
       <c r="G51" s="6"/>
       <c r="H51" s="6"/>
       <c r="I51" s="6"/>
@@ -2326,20 +2404,22 @@
       <c r="O51" s="6"/>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A52" s="10"/>
+      <c r="A52" s="8">
+        <v>13</v>
+      </c>
       <c r="B52" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C52" s="11" t="s">
-        <v>105</v>
+        <v>107</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="F52" s="5"/>
+        <v>46</v>
+      </c>
+      <c r="F52" s="6"/>
       <c r="G52" s="6"/>
       <c r="H52" s="6"/>
       <c r="I52" s="6"/>
@@ -2351,20 +2431,22 @@
       <c r="O52" s="6"/>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A53" s="10"/>
+      <c r="A53" s="8">
+        <v>13</v>
+      </c>
       <c r="B53" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C53" s="11" t="s">
-        <v>104</v>
+        <v>107</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>81</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="F53" s="5"/>
+        <v>102</v>
+      </c>
+      <c r="F53" s="6"/>
       <c r="G53" s="6"/>
       <c r="H53" s="6"/>
       <c r="I53" s="6"/>
@@ -2376,20 +2458,22 @@
       <c r="O53" s="6"/>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A54" s="10"/>
+      <c r="A54" s="8">
+        <v>16</v>
+      </c>
       <c r="B54" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C54" s="11" t="s">
-        <v>104</v>
+        <v>108</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="F54" s="5"/>
+        <v>30</v>
+      </c>
+      <c r="F54" s="6"/>
       <c r="G54" s="6"/>
       <c r="H54" s="6"/>
       <c r="I54" s="6"/>
@@ -2401,20 +2485,22 @@
       <c r="O54" s="6"/>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A55" s="10"/>
+      <c r="A55" s="8">
+        <v>16</v>
+      </c>
       <c r="B55" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C55" s="11" t="s">
-        <v>104</v>
+        <v>108</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F55" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="F55" s="6"/>
       <c r="G55" s="6"/>
       <c r="H55" s="6"/>
       <c r="I55" s="6"/>
@@ -2426,20 +2512,22 @@
       <c r="O55" s="6"/>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A56" s="10"/>
+      <c r="A56" s="8">
+        <v>16</v>
+      </c>
       <c r="B56" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C56" s="11" t="s">
-        <v>104</v>
+        <v>108</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="F56" s="5"/>
+        <v>32</v>
+      </c>
+      <c r="F56" s="6"/>
       <c r="G56" s="6"/>
       <c r="H56" s="6"/>
       <c r="I56" s="6"/>
@@ -2451,20 +2539,20 @@
       <c r="O56" s="6"/>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A57" s="10"/>
+      <c r="A57" s="8">
+        <v>16</v>
+      </c>
       <c r="B57" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C57" s="11" t="s">
-        <v>104</v>
+        <v>108</v>
+      </c>
+      <c r="C57" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="F57" s="5"/>
+        <v>66</v>
+      </c>
+      <c r="E57" s="3"/>
+      <c r="F57" s="6"/>
       <c r="G57" s="6"/>
       <c r="H57" s="6"/>
       <c r="I57" s="6"/>
@@ -2476,20 +2564,22 @@
       <c r="O57" s="6"/>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A58" s="10"/>
+      <c r="A58" s="8">
+        <v>16</v>
+      </c>
       <c r="B58" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C58" s="11" t="s">
-        <v>104</v>
+        <v>108</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F58" s="5"/>
+        <v>33</v>
+      </c>
+      <c r="F58" s="6"/>
       <c r="G58" s="6"/>
       <c r="H58" s="6"/>
       <c r="I58" s="6"/>
@@ -2501,20 +2591,22 @@
       <c r="O58" s="6"/>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A59" s="10"/>
+      <c r="A59" s="8">
+        <v>16</v>
+      </c>
       <c r="B59" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C59" s="11" t="s">
-        <v>104</v>
+        <v>108</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="F59" s="5"/>
+        <v>34</v>
+      </c>
+      <c r="F59" s="6"/>
       <c r="G59" s="6"/>
       <c r="H59" s="6"/>
       <c r="I59" s="6"/>
@@ -2526,20 +2618,22 @@
       <c r="O59" s="6"/>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A60" s="10"/>
+      <c r="A60" s="8">
+        <v>16</v>
+      </c>
       <c r="B60" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C60" s="11" t="s">
-        <v>104</v>
+        <v>108</v>
+      </c>
+      <c r="C60" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="F60" s="5"/>
+        <v>35</v>
+      </c>
+      <c r="F60" s="6"/>
       <c r="G60" s="6"/>
       <c r="H60" s="6"/>
       <c r="I60" s="6"/>
@@ -2551,16 +2645,22 @@
       <c r="O60" s="6"/>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A61" s="10"/>
-      <c r="B61" s="2"/>
-      <c r="C61" s="11" t="s">
-        <v>104</v>
+      <c r="A61" s="8">
+        <v>16</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="E61" s="3"/>
-      <c r="F61" s="5"/>
+        <v>67</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F61" s="6"/>
       <c r="G61" s="6"/>
       <c r="H61" s="6"/>
       <c r="I61" s="6"/>
@@ -2572,16 +2672,22 @@
       <c r="O61" s="6"/>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A62" s="10"/>
-      <c r="B62" s="2"/>
-      <c r="C62" s="11" t="s">
-        <v>104</v>
+      <c r="A62" s="8">
+        <v>16</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="E62" s="3"/>
-      <c r="F62" s="5"/>
+        <v>67</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F62" s="6"/>
       <c r="G62" s="6"/>
       <c r="H62" s="6"/>
       <c r="I62" s="6"/>
@@ -2593,16 +2699,22 @@
       <c r="O62" s="6"/>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A63" s="10"/>
-      <c r="B63" s="2"/>
-      <c r="C63" s="11" t="s">
-        <v>104</v>
+      <c r="A63" s="8">
+        <v>17</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C63" s="9" t="s">
+        <v>81</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="E63" s="3"/>
-      <c r="F63" s="5"/>
+        <v>67</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F63" s="6"/>
       <c r="G63" s="6"/>
       <c r="H63" s="6"/>
       <c r="I63" s="6"/>
@@ -2614,16 +2726,22 @@
       <c r="O63" s="6"/>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A64" s="10"/>
-      <c r="B64" s="2"/>
-      <c r="C64" s="11" t="s">
-        <v>104</v>
+      <c r="A64" s="8">
+        <v>17</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C64" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="E64" s="3"/>
-      <c r="F64" s="5"/>
+        <v>67</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F64" s="6"/>
       <c r="G64" s="6"/>
       <c r="H64" s="6"/>
       <c r="I64" s="6"/>
@@ -2635,16 +2753,22 @@
       <c r="O64" s="6"/>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A65" s="10"/>
-      <c r="B65" s="2"/>
-      <c r="C65" s="11" t="s">
-        <v>104</v>
+      <c r="A65" s="8">
+        <v>17</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C65" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="E65" s="3"/>
-      <c r="F65" s="5"/>
+        <v>66</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F65" s="6"/>
       <c r="G65" s="6"/>
       <c r="H65" s="6"/>
       <c r="I65" s="6"/>
@@ -2656,16 +2780,22 @@
       <c r="O65" s="6"/>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A66" s="10"/>
-      <c r="B66" s="2"/>
-      <c r="C66" s="11" t="s">
-        <v>104</v>
+      <c r="A66" s="8">
+        <v>17</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C66" s="9" t="s">
+        <v>81</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="E66" s="3"/>
-      <c r="F66" s="5"/>
+        <v>66</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F66" s="6"/>
       <c r="G66" s="6"/>
       <c r="H66" s="6"/>
       <c r="I66" s="6"/>
@@ -2677,16 +2807,22 @@
       <c r="O66" s="6"/>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A67" s="10"/>
-      <c r="B67" s="2"/>
-      <c r="C67" s="11" t="s">
-        <v>104</v>
+      <c r="A67" s="8">
+        <v>20</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C67" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="E67" s="3"/>
-      <c r="F67" s="5"/>
+        <v>67</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F67" s="6"/>
       <c r="G67" s="6"/>
       <c r="H67" s="6"/>
       <c r="I67" s="6"/>
@@ -2698,16 +2834,22 @@
       <c r="O67" s="6"/>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A68" s="10"/>
-      <c r="B68" s="2"/>
-      <c r="C68" s="11" t="s">
-        <v>104</v>
+      <c r="A68" s="8">
+        <v>20</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C68" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="E68" s="3"/>
-      <c r="F68" s="5"/>
+        <v>66</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F68" s="6"/>
       <c r="G68" s="6"/>
       <c r="H68" s="6"/>
       <c r="I68" s="6"/>
@@ -2719,16 +2861,22 @@
       <c r="O68" s="6"/>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A69" s="10"/>
-      <c r="B69" s="2"/>
-      <c r="C69" s="11" t="s">
-        <v>104</v>
+      <c r="A69" s="8">
+        <v>20</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C69" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="E69" s="3"/>
-      <c r="F69" s="5"/>
+        <v>66</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F69" s="6"/>
       <c r="G69" s="6"/>
       <c r="H69" s="6"/>
       <c r="I69" s="6"/>
@@ -2738,6 +2886,145 @@
       <c r="M69" s="6"/>
       <c r="N69" s="6"/>
       <c r="O69" s="6"/>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A70" s="8">
+        <v>20</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C70" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F70" s="6"/>
+      <c r="G70" s="6"/>
+      <c r="H70" s="6"/>
+      <c r="I70" s="6"/>
+      <c r="J70" s="6"/>
+      <c r="K70" s="6"/>
+      <c r="L70" s="6"/>
+      <c r="M70" s="6"/>
+      <c r="N70" s="6"/>
+      <c r="O70" s="6"/>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A71" s="8">
+        <v>20</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C71" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F71" s="6"/>
+      <c r="G71" s="6"/>
+      <c r="H71" s="6"/>
+      <c r="I71" s="6"/>
+      <c r="J71" s="6"/>
+      <c r="K71" s="6"/>
+      <c r="L71" s="6"/>
+      <c r="M71" s="6"/>
+      <c r="N71" s="6"/>
+      <c r="O71" s="6"/>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A72" s="8"/>
+      <c r="B72" s="2"/>
+      <c r="C72" s="9"/>
+      <c r="D72" s="5"/>
+      <c r="E72" s="3"/>
+      <c r="F72" s="6"/>
+      <c r="G72" s="6"/>
+      <c r="H72" s="6"/>
+      <c r="I72" s="6"/>
+      <c r="J72" s="6"/>
+      <c r="K72" s="6"/>
+      <c r="L72" s="6"/>
+      <c r="M72" s="6"/>
+      <c r="N72" s="6"/>
+      <c r="O72" s="6"/>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A73" s="8"/>
+      <c r="B73" s="2"/>
+      <c r="C73" s="9"/>
+      <c r="D73" s="5"/>
+      <c r="E73" s="3"/>
+      <c r="F73" s="6"/>
+      <c r="G73" s="6"/>
+      <c r="H73" s="6"/>
+      <c r="I73" s="6"/>
+      <c r="J73" s="6"/>
+      <c r="K73" s="6"/>
+      <c r="L73" s="6"/>
+      <c r="M73" s="6"/>
+      <c r="N73" s="6"/>
+      <c r="O73" s="6"/>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A74" s="8"/>
+      <c r="B74" s="2"/>
+      <c r="C74" s="9"/>
+      <c r="D74" s="5"/>
+      <c r="E74" s="3"/>
+      <c r="F74" s="6"/>
+      <c r="G74" s="6"/>
+      <c r="H74" s="6"/>
+      <c r="I74" s="6"/>
+      <c r="J74" s="6"/>
+      <c r="K74" s="6"/>
+      <c r="L74" s="6"/>
+      <c r="M74" s="6"/>
+      <c r="N74" s="6"/>
+      <c r="O74" s="6"/>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A75" s="8"/>
+      <c r="B75" s="2"/>
+      <c r="C75" s="9"/>
+      <c r="D75" s="5"/>
+      <c r="E75" s="3"/>
+      <c r="F75" s="6"/>
+      <c r="G75" s="6"/>
+      <c r="H75" s="6"/>
+      <c r="I75" s="6"/>
+      <c r="J75" s="6"/>
+      <c r="K75" s="6"/>
+      <c r="L75" s="6"/>
+      <c r="M75" s="6"/>
+      <c r="N75" s="6"/>
+      <c r="O75" s="6"/>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A76" s="8"/>
+      <c r="B76" s="2"/>
+      <c r="C76" s="9"/>
+      <c r="D76" s="5"/>
+      <c r="E76" s="3"/>
+      <c r="F76" s="6"/>
+      <c r="G76" s="6"/>
+      <c r="H76" s="6"/>
+      <c r="I76" s="6"/>
+      <c r="J76" s="6"/>
+      <c r="K76" s="6"/>
+      <c r="L76" s="6"/>
+      <c r="M76" s="6"/>
+      <c r="N76" s="6"/>
+      <c r="O76" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2758,13 +3045,13 @@
           <x14:formula1>
             <xm:f>Info!$A$2:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>G3:O69</xm:sqref>
+          <xm:sqref>F3:O76</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F57E977A-DCE3-453D-B6A7-FAA0E0182939}">
           <x14:formula1>
             <xm:f>Info!$B$2:$B$6</xm:f>
           </x14:formula1>
-          <xm:sqref>C3:C69</xm:sqref>
+          <xm:sqref>C3:C76</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2788,35 +3075,35 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>114</v>
+        <v>89</v>
       </c>
       <c r="B1" t="s">
-        <v>115</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>87</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -2843,47 +3130,47 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="B1" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>97</v>
+        <v>73</v>
       </c>
       <c r="B3" t="s">
-        <v>105</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>96</v>
+        <v>72</v>
       </c>
       <c r="B4" t="s">
-        <v>106</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>98</v>
+        <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>94</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>